<commit_message>
fix: updated part number for SW1
</commit_message>
<xml_diff>
--- a/output/bom.xlsx
+++ b/output/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/padmal/Desktop/FOSSASIA/badgemagic-hardware/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F5CAE9-22D8-2947-B5D1-DFF3F8FDECCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6320B696-E347-834C-BD16-DE63037F67DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="480" windowWidth="14200" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14600" yWindow="500" windowWidth="14200" windowHeight="15620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>C5159679</t>
   </si>
   <si>
-    <t>C18078237</t>
-  </si>
-  <si>
     <t>JST_1x02_P2.50mm_SMD_Horizontal</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>Crystal_SMD_2016-4Pin_2.0x1.6mm</t>
   </si>
   <si>
-    <t>SW_DIP_SPSTx01_Slide_Copal_CHS-01A_W5.08mm_P1.27mm_JPin</t>
-  </si>
-  <si>
     <t>Conn_01x02</t>
   </si>
   <si>
@@ -281,6 +275,12 @@
   </si>
   <si>
     <t>D401,D402,D403,D404,D405,D406,D407,D408,D409,D410,D411,D412,D413,D414,D415,D416,D417,D418,D419,D420,D421,D422,D423,D424,D425,D426,D427,D428,D429,D430,D431,D432,D433,D434,D435,D436,D437,D438,D439,D440,D441,D442,D443,D444,D445,D446,D447,D448,D449,D450,D451,D452,D453,D454,D455,D456,D457,D458,D459,D460,D461,D462,D463,D464,D465,D466,D467,D468,D469,D470,D471,D472,D473,D474,D475,D476,D477,D478,D479,D480,D481,D482,D483,D484</t>
+  </si>
+  <si>
+    <t>C2921603</t>
+  </si>
+  <si>
+    <t>SW_DIP_SPSTx01_Slide_Copal_CHS-01TA_W5.08mm_P1.27mm_Jpin</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
@@ -732,7 +732,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -740,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
@@ -754,7 +754,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
@@ -768,7 +768,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>6</v>
@@ -782,7 +782,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
@@ -796,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
@@ -807,13 +807,13 @@
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
@@ -821,13 +821,13 @@
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>9</v>
@@ -835,13 +835,13 @@
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>10</v>
@@ -849,13 +849,13 @@
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>11</v>
@@ -863,13 +863,13 @@
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
@@ -877,13 +877,13 @@
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>13</v>
@@ -891,13 +891,13 @@
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>14</v>
@@ -905,13 +905,13 @@
     </row>
     <row r="14" spans="1:4" ht="20" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>15</v>
@@ -919,13 +919,13 @@
     </row>
     <row r="15" spans="1:4" ht="20" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>16</v>
@@ -933,13 +933,13 @@
     </row>
     <row r="16" spans="1:4" ht="20" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>17</v>
@@ -947,13 +947,13 @@
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>18</v>
@@ -961,13 +961,13 @@
     </row>
     <row r="18" spans="1:4" ht="20" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>19</v>
@@ -975,13 +975,13 @@
     </row>
     <row r="19" spans="1:4" ht="20" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>20</v>
@@ -989,13 +989,13 @@
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>21</v>
@@ -1003,13 +1003,13 @@
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>22</v>
@@ -1017,13 +1017,13 @@
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>23</v>
@@ -1031,13 +1031,13 @@
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>24</v>
@@ -1045,13 +1045,13 @@
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>25</v>
@@ -1059,13 +1059,13 @@
     </row>
     <row r="25" spans="1:4" ht="20" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>26</v>
@@ -1073,13 +1073,13 @@
     </row>
     <row r="26" spans="1:4" ht="20" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>27</v>
@@ -1087,16 +1087,16 @@
     </row>
     <row r="27" spans="1:4" ht="20" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: updated part number for SW1 (#40)
</commit_message>
<xml_diff>
--- a/output/bom.xlsx
+++ b/output/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/padmal/Desktop/FOSSASIA/badgemagic-hardware/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F5CAE9-22D8-2947-B5D1-DFF3F8FDECCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6320B696-E347-834C-BD16-DE63037F67DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="480" windowWidth="14200" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14600" yWindow="500" windowWidth="14200" windowHeight="15620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>C5159679</t>
   </si>
   <si>
-    <t>C18078237</t>
-  </si>
-  <si>
     <t>JST_1x02_P2.50mm_SMD_Horizontal</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>Crystal_SMD_2016-4Pin_2.0x1.6mm</t>
   </si>
   <si>
-    <t>SW_DIP_SPSTx01_Slide_Copal_CHS-01A_W5.08mm_P1.27mm_JPin</t>
-  </si>
-  <si>
     <t>Conn_01x02</t>
   </si>
   <si>
@@ -281,6 +275,12 @@
   </si>
   <si>
     <t>D401,D402,D403,D404,D405,D406,D407,D408,D409,D410,D411,D412,D413,D414,D415,D416,D417,D418,D419,D420,D421,D422,D423,D424,D425,D426,D427,D428,D429,D430,D431,D432,D433,D434,D435,D436,D437,D438,D439,D440,D441,D442,D443,D444,D445,D446,D447,D448,D449,D450,D451,D452,D453,D454,D455,D456,D457,D458,D459,D460,D461,D462,D463,D464,D465,D466,D467,D468,D469,D470,D471,D472,D473,D474,D475,D476,D477,D478,D479,D480,D481,D482,D483,D484</t>
+  </si>
+  <si>
+    <t>C2921603</t>
+  </si>
+  <si>
+    <t>SW_DIP_SPSTx01_Slide_Copal_CHS-01TA_W5.08mm_P1.27mm_Jpin</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
@@ -732,7 +732,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1">
@@ -740,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
@@ -754,7 +754,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
@@ -768,7 +768,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>6</v>
@@ -782,7 +782,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
@@ -796,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
@@ -807,13 +807,13 @@
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
@@ -821,13 +821,13 @@
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>9</v>
@@ -835,13 +835,13 @@
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>10</v>
@@ -849,13 +849,13 @@
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>11</v>
@@ -863,13 +863,13 @@
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
@@ -877,13 +877,13 @@
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>13</v>
@@ -891,13 +891,13 @@
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>14</v>
@@ -905,13 +905,13 @@
     </row>
     <row r="14" spans="1:4" ht="20" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>15</v>
@@ -919,13 +919,13 @@
     </row>
     <row r="15" spans="1:4" ht="20" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>16</v>
@@ -933,13 +933,13 @@
     </row>
     <row r="16" spans="1:4" ht="20" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>17</v>
@@ -947,13 +947,13 @@
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>18</v>
@@ -961,13 +961,13 @@
     </row>
     <row r="18" spans="1:4" ht="20" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>19</v>
@@ -975,13 +975,13 @@
     </row>
     <row r="19" spans="1:4" ht="20" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>20</v>
@@ -989,13 +989,13 @@
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>21</v>
@@ -1003,13 +1003,13 @@
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>22</v>
@@ -1017,13 +1017,13 @@
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>23</v>
@@ -1031,13 +1031,13 @@
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>24</v>
@@ -1045,13 +1045,13 @@
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>25</v>
@@ -1059,13 +1059,13 @@
     </row>
     <row r="25" spans="1:4" ht="20" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>26</v>
@@ -1073,13 +1073,13 @@
     </row>
     <row r="26" spans="1:4" ht="20" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>27</v>
@@ -1087,16 +1087,16 @@
     </row>
     <row r="27" spans="1:4" ht="20" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>